<commit_message>
worked on the employee module
</commit_message>
<xml_diff>
--- a/src/test/resources/student_registration.xlsx
+++ b/src/test/resources/student_registration.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="176">
   <si>
     <t>India</t>
   </si>
@@ -555,7 +555,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="38" x14ac:knownFonts="1">
+  <fonts count="42" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -694,6 +694,26 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1173,7 +1193,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1260,6 +1280,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1773,364 +1809,364 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:123" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="41" t="s">
+      <c r="D1" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="41" t="s">
+      <c r="E1" s="49" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="49" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="41" t="s">
+      <c r="G1" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="41" t="s">
+      <c r="H1" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="49" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="49" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="41" t="s">
+      <c r="K1" s="49" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="41" t="s">
+      <c r="L1" s="49" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="41" t="s">
+      <c r="M1" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="49" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="41" t="s">
+      <c r="O1" s="49" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="41" t="s">
+      <c r="P1" s="49" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="41" t="s">
+      <c r="Q1" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="41" t="s">
+      <c r="R1" s="49" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="41" t="s">
+      <c r="S1" s="49" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="41" t="s">
+      <c r="T1" s="49" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="41" t="s">
+      <c r="U1" s="49" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="41" t="s">
+      <c r="V1" s="49" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="41" t="s">
+      <c r="W1" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="41" t="s">
+      <c r="X1" s="49" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="41" t="s">
+      <c r="Y1" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="41" t="s">
+      <c r="Z1" s="49" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="41" t="s">
+      <c r="AB1" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="41" t="s">
+      <c r="AC1" s="49" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="41" t="s">
+      <c r="AD1" s="49" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="41" t="s">
+      <c r="AE1" s="49" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="41" t="s">
+      <c r="AF1" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="41" t="s">
+      <c r="AG1" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="AH1" s="41" t="s">
+      <c r="AH1" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" s="41" t="s">
+      <c r="AI1" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="AJ1" s="41" t="s">
+      <c r="AJ1" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="AK1" s="41" t="s">
+      <c r="AK1" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="AL1" s="41" t="s">
+      <c r="AL1" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="AM1" s="41" t="s">
+      <c r="AM1" s="49" t="s">
         <v>43</v>
       </c>
-      <c r="AN1" s="41" t="s">
+      <c r="AN1" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="AO1" s="41" t="s">
+      <c r="AO1" s="49" t="s">
         <v>45</v>
       </c>
-      <c r="AP1" s="41" t="s">
+      <c r="AP1" s="49" t="s">
         <v>46</v>
       </c>
-      <c r="AQ1" s="41" t="s">
+      <c r="AQ1" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="AR1" s="41" t="s">
+      <c r="AR1" s="49" t="s">
         <v>48</v>
       </c>
-      <c r="AS1" s="41" t="s">
+      <c r="AS1" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="AT1" s="41" t="s">
+      <c r="AT1" s="49" t="s">
         <v>50</v>
       </c>
-      <c r="AU1" s="41" t="s">
+      <c r="AU1" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="AV1" s="41" t="s">
+      <c r="AV1" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="AW1" s="41" t="s">
+      <c r="AW1" s="49" t="s">
         <v>53</v>
       </c>
-      <c r="AX1" s="41" t="s">
+      <c r="AX1" s="49" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" s="41" t="s">
+      <c r="AY1" s="49" t="s">
         <v>55</v>
       </c>
-      <c r="AZ1" s="41" t="s">
+      <c r="AZ1" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="BA1" s="41" t="s">
+      <c r="BA1" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="BB1" s="41" t="s">
+      <c r="BB1" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" s="41" t="s">
+      <c r="BC1" s="49" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="41" t="s">
+      <c r="BD1" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" s="41" t="s">
+      <c r="BE1" s="49" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="41" t="s">
+      <c r="BF1" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="41" t="s">
+      <c r="BG1" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="41" t="s">
+      <c r="BH1" s="49" t="s">
         <v>64</v>
       </c>
-      <c r="BI1" s="41" t="s">
+      <c r="BI1" s="49" t="s">
         <v>65</v>
       </c>
-      <c r="BJ1" s="41" t="s">
+      <c r="BJ1" s="49" t="s">
         <v>66</v>
       </c>
-      <c r="BK1" s="41" t="s">
+      <c r="BK1" s="49" t="s">
         <v>67</v>
       </c>
-      <c r="BL1" s="41" t="s">
+      <c r="BL1" s="49" t="s">
         <v>68</v>
       </c>
-      <c r="BM1" s="41" t="s">
+      <c r="BM1" s="49" t="s">
         <v>69</v>
       </c>
-      <c r="BN1" s="41" t="s">
+      <c r="BN1" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="BO1" s="41" t="s">
+      <c r="BO1" s="49" t="s">
         <v>71</v>
       </c>
-      <c r="BP1" s="41" t="s">
+      <c r="BP1" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="BQ1" s="41" t="s">
+      <c r="BQ1" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="BR1" s="41" t="s">
+      <c r="BR1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="BS1" s="41" t="s">
+      <c r="BS1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="BT1" s="41" t="s">
+      <c r="BT1" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="BU1" s="41" t="s">
+      <c r="BU1" s="49" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="41" t="s">
+      <c r="BV1" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="41" t="s">
+      <c r="BW1" s="49" t="s">
         <v>79</v>
       </c>
-      <c r="BX1" s="41" t="s">
+      <c r="BX1" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="BY1" s="41" t="s">
+      <c r="BY1" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="BZ1" s="41" t="s">
+      <c r="BZ1" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="CA1" s="41" t="s">
+      <c r="CA1" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="CB1" s="41" t="s">
+      <c r="CB1" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="CC1" s="41" t="s">
+      <c r="CC1" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="CD1" s="41" t="s">
+      <c r="CD1" s="49" t="s">
         <v>86</v>
       </c>
-      <c r="CE1" s="41" t="s">
+      <c r="CE1" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="CF1" s="41" t="s">
+      <c r="CF1" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="CG1" s="41" t="s">
+      <c r="CG1" s="49" t="s">
         <v>89</v>
       </c>
-      <c r="CH1" s="41" t="s">
+      <c r="CH1" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="CI1" s="41" t="s">
+      <c r="CI1" s="49" t="s">
         <v>91</v>
       </c>
-      <c r="CJ1" s="41" t="s">
+      <c r="CJ1" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="CK1" s="41" t="s">
+      <c r="CK1" s="49" t="s">
         <v>93</v>
       </c>
-      <c r="CL1" s="41" t="s">
+      <c r="CL1" s="49" t="s">
         <v>94</v>
       </c>
-      <c r="CM1" s="41" t="s">
+      <c r="CM1" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="CN1" s="41" t="s">
+      <c r="CN1" s="49" t="s">
         <v>96</v>
       </c>
-      <c r="CO1" s="41" t="s">
+      <c r="CO1" s="49" t="s">
         <v>97</v>
       </c>
-      <c r="CP1" s="41" t="s">
+      <c r="CP1" s="49" t="s">
         <v>98</v>
       </c>
-      <c r="CQ1" s="41" t="s">
+      <c r="CQ1" s="49" t="s">
         <v>99</v>
       </c>
-      <c r="CR1" s="41" t="s">
+      <c r="CR1" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="CS1" s="41" t="s">
+      <c r="CS1" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="CT1" s="41" t="s">
+      <c r="CT1" s="49" t="s">
         <v>102</v>
       </c>
-      <c r="CU1" s="41" t="s">
+      <c r="CU1" s="49" t="s">
         <v>103</v>
       </c>
-      <c r="CV1" s="41" t="s">
+      <c r="CV1" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="CW1" s="41" t="s">
+      <c r="CW1" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="CX1" s="41" t="s">
+      <c r="CX1" s="49" t="s">
         <v>104</v>
       </c>
-      <c r="CY1" s="41" t="s">
+      <c r="CY1" s="49" t="s">
         <v>105</v>
       </c>
-      <c r="CZ1" s="41" t="s">
+      <c r="CZ1" s="49" t="s">
         <v>106</v>
       </c>
-      <c r="DA1" s="41" t="s">
+      <c r="DA1" s="49" t="s">
         <v>107</v>
       </c>
-      <c r="DB1" s="41" t="s">
+      <c r="DB1" s="49" t="s">
         <v>108</v>
       </c>
-      <c r="DC1" s="41" t="s">
+      <c r="DC1" s="49" t="s">
         <v>109</v>
       </c>
-      <c r="DD1" s="41" t="s">
+      <c r="DD1" s="49" t="s">
         <v>110</v>
       </c>
-      <c r="DE1" s="41" t="s">
+      <c r="DE1" s="49" t="s">
         <v>111</v>
       </c>
-      <c r="DF1" s="41" t="s">
+      <c r="DF1" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="DG1" s="41" t="s">
+      <c r="DG1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="DH1" s="41" t="s">
+      <c r="DH1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="DI1" s="41" t="s">
+      <c r="DI1" s="49" t="s">
         <v>115</v>
       </c>
-      <c r="DJ1" s="41" t="s">
+      <c r="DJ1" s="49" t="s">
         <v>116</v>
       </c>
-      <c r="DK1" s="41" t="s">
+      <c r="DK1" s="49" t="s">
         <v>117</v>
       </c>
-      <c r="DL1" s="41" t="s">
+      <c r="DL1" s="49" t="s">
         <v>118</v>
       </c>
-      <c r="DM1" s="41" t="s">
+      <c r="DM1" s="49" t="s">
         <v>119</v>
       </c>
-      <c r="DN1" s="41" t="s">
+      <c r="DN1" s="49" t="s">
         <v>120</v>
       </c>
-      <c r="DO1" s="41" t="s">
+      <c r="DO1" s="49" t="s">
         <v>121</v>
       </c>
-      <c r="DP1" s="41" t="s">
+      <c r="DP1" s="49" t="s">
         <v>122</v>
       </c>
       <c r="DQ1" s="4" t="s">
@@ -2498,7 +2534,7 @@
       <c r="DN2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="DO2" s="42" t="s">
+      <c r="DO2" s="50" t="s">
         <v>172</v>
       </c>
       <c r="DP2" s="2">

</xml_diff>

<commit_message>
Changed in All file
</commit_message>
<xml_diff>
--- a/src/test/resources/student_registration.xlsx
+++ b/src/test/resources/student_registration.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Automation\com.ihsm.university.project\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ismedusoftsol-my.sharepoint.com/personal/ajangra_ismedusoftsol_com/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4973000A-A087-4DBD-8E7C-68886CF9E153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{63123A0B-69EF-4957-A449-3D785EBC22EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CFD072B-9663-4C55-A81C-BACEC5719E8D}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{83E1AD02-E6B5-41C8-98D7-77709091ACEC}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="177">
   <si>
     <t>India</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Diploma</t>
   </si>
   <si>
-    <t>English</t>
-  </si>
-  <si>
     <t>Term</t>
   </si>
   <si>
@@ -410,6 +407,15 @@
     <t>PIN1000</t>
   </si>
   <si>
+    <t>First</t>
+  </si>
+  <si>
+    <t>Middle</t>
+  </si>
+  <si>
+    <t>Last</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -428,33 +434,15 @@
     <t>Panipat</t>
   </si>
   <si>
-    <t>Single</t>
-  </si>
-  <si>
     <t>male.png</t>
   </si>
   <si>
-    <t>Father</t>
-  </si>
-  <si>
     <t>Mukesh Kumar</t>
   </si>
   <si>
-    <t>Business</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
-    <t>B2</t>
-  </si>
-  <si>
-    <t>rights</t>
-  </si>
-  <si>
-    <t>value</t>
-  </si>
-  <si>
     <t>dose 1</t>
   </si>
   <si>
@@ -473,9 +461,6 @@
     <t>ID12345</t>
   </si>
   <si>
-    <t>11 Months Double</t>
-  </si>
-  <si>
     <t>Home Country</t>
   </si>
   <si>
@@ -485,9 +470,6 @@
     <t>No Remarks</t>
   </si>
   <si>
-    <t>14 Month Single</t>
-  </si>
-  <si>
     <t>OVNP1234</t>
   </si>
   <si>
@@ -542,13 +524,34 @@
     <t>Enrolled and Active</t>
   </si>
   <si>
-    <t>Rohit</t>
-  </si>
-  <si>
-    <t>Kumar</t>
-  </si>
-  <si>
-    <t>Sharma</t>
+    <t>Nothing</t>
+  </si>
+  <si>
+    <t>Brother</t>
+  </si>
+  <si>
+    <t>Textile Industry Owner</t>
+  </si>
+  <si>
+    <t>Mandarian</t>
+  </si>
+  <si>
+    <t>Level 1</t>
+  </si>
+  <si>
+    <t>Add Rights Here</t>
+  </si>
+  <si>
+    <t>Add Social Status Here</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>H1_B Visa</t>
+  </si>
+  <si>
+    <t>H1_B Online Visa</t>
   </si>
 </sst>
 </file>
@@ -556,7 +559,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="40" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -695,6 +698,91 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <b val="true"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -1099,7 +1187,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1126,6 +1214,74 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="38" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="35" borderId="0" xfId="0" applyFont="true" applyFill="true"/>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="10" xfId="0" applyBorder="1" applyAlignment="1" applyFill="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1185,6 +1341,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1506,7 +1666,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B341502D-6CB3-4F48-AED9-FE9E3EEFEF78}">
   <dimension ref="A1:DS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BI1" workbookViewId="0">
       <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft"/>
     </sheetView>
@@ -1537,7 +1697,7 @@
     <col min="22" max="22" bestFit="true" customWidth="true" width="7.10546875"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="13.00390625"/>
     <col min="24" max="24" bestFit="true" customWidth="true" width="9.1328125"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="9.3984375"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.90234375"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="10.61328125"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="9.9140625"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="9.1953125"/>
@@ -1545,11 +1705,11 @@
     <col min="30" max="30" bestFit="true" customWidth="true" width="12.00390625"/>
     <col min="31" max="31" bestFit="true" customWidth="true" width="7.01171875"/>
     <col min="32" max="32" bestFit="true" customWidth="true" width="12.3515625"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="7.9375"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="9.41015625"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="11.80078125"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="7.9765625"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="14.10546875"/>
     <col min="36" max="36" bestFit="true" customWidth="true" width="12.5625"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="9.87109375"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="19.50390625"/>
     <col min="38" max="38" bestFit="true" customWidth="true" width="14.45703125"/>
     <col min="39" max="39" bestFit="true" customWidth="true" width="15.9140625"/>
     <col min="40" max="40" bestFit="true" customWidth="true" width="7.2890625"/>
@@ -1575,7 +1735,7 @@
     <col min="60" max="60" bestFit="true" customWidth="true" width="9.640625"/>
     <col min="61" max="61" bestFit="true" customWidth="true" width="10.45703125"/>
     <col min="62" max="62" bestFit="true" customWidth="true" width="7.7109375"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="15.5078125"/>
+    <col min="63" max="63" bestFit="true" customWidth="true" width="9.41015625"/>
     <col min="64" max="64" bestFit="true" customWidth="true" width="13.484375"/>
     <col min="65" max="65" bestFit="true" customWidth="true" width="11.30859375"/>
     <col min="66" max="66" bestFit="true" customWidth="true" width="11.14453125"/>
@@ -1585,7 +1745,7 @@
     <col min="70" max="70" bestFit="true" customWidth="true" width="9.93359375"/>
     <col min="71" max="71" bestFit="true" customWidth="true" width="10.90625"/>
     <col min="72" max="72" bestFit="true" customWidth="true" width="8.55859375"/>
-    <col min="73" max="73" bestFit="true" customWidth="true" width="13.91015625"/>
+    <col min="73" max="73" bestFit="true" customWidth="true" width="15.10546875"/>
     <col min="74" max="74" bestFit="true" customWidth="true" width="16.08203125"/>
     <col min="75" max="75" bestFit="true" customWidth="true" width="16.2421875"/>
     <col min="76" max="76" bestFit="true" customWidth="true" width="15.26171875"/>
@@ -1639,382 +1799,382 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:123" ht="36" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="45" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="C1" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="E1" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="H1" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="I1" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="11" t="s">
+      <c r="L1" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="11" t="s">
+      <c r="M1" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="11" t="s">
+      <c r="N1" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="O1" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="11" t="s">
+      <c r="P1" s="45" t="s">
         <v>20</v>
       </c>
-      <c r="P1" s="11" t="s">
+      <c r="Q1" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="Q1" s="11" t="s">
+      <c r="R1" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="R1" s="11" t="s">
+      <c r="S1" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="S1" s="11" t="s">
+      <c r="T1" s="45" t="s">
         <v>24</v>
       </c>
-      <c r="T1" s="11" t="s">
+      <c r="U1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="V1" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="V1" s="11" t="s">
+      <c r="W1" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="W1" s="11" t="s">
+      <c r="X1" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="X1" s="11" t="s">
+      <c r="Y1" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="Y1" s="11" t="s">
+      <c r="Z1" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="Z1" s="11" t="s">
+      <c r="AA1" s="45" t="s">
         <v>31</v>
       </c>
-      <c r="AA1" s="11" t="s">
+      <c r="AB1" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="AB1" s="11" t="s">
+      <c r="AC1" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="AC1" s="11" t="s">
+      <c r="AD1" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="AD1" s="11" t="s">
+      <c r="AE1" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="AE1" s="11" t="s">
+      <c r="AF1" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="AF1" s="11" t="s">
+      <c r="AG1" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="AH1" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="AG1" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="AH1" s="11" t="s">
+      <c r="AI1" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" s="11" t="s">
+      <c r="AJ1" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="AJ1" s="11" t="s">
+      <c r="AK1" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="AK1" s="11" t="s">
+      <c r="AL1" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="AL1" s="11" t="s">
+      <c r="AM1" s="45" t="s">
         <v>42</v>
       </c>
-      <c r="AM1" s="11" t="s">
+      <c r="AN1" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="AN1" s="11" t="s">
+      <c r="AO1" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="AO1" s="11" t="s">
+      <c r="AP1" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="AP1" s="11" t="s">
+      <c r="AQ1" s="45" t="s">
         <v>46</v>
       </c>
-      <c r="AQ1" s="11" t="s">
+      <c r="AR1" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="AR1" s="11" t="s">
+      <c r="AS1" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="AS1" s="11" t="s">
+      <c r="AT1" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="AT1" s="11" t="s">
+      <c r="AU1" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="AU1" s="11" t="s">
+      <c r="AV1" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="AV1" s="11" t="s">
+      <c r="AW1" s="45" t="s">
         <v>52</v>
       </c>
-      <c r="AW1" s="11" t="s">
+      <c r="AX1" s="45" t="s">
         <v>53</v>
       </c>
-      <c r="AX1" s="11" t="s">
+      <c r="AY1" s="45" t="s">
         <v>54</v>
       </c>
-      <c r="AY1" s="11" t="s">
+      <c r="AZ1" s="45" t="s">
         <v>55</v>
       </c>
-      <c r="AZ1" s="11" t="s">
+      <c r="BA1" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="BA1" s="11" t="s">
+      <c r="BB1" s="45" t="s">
         <v>57</v>
       </c>
-      <c r="BB1" s="11" t="s">
+      <c r="BC1" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="BC1" s="11" t="s">
+      <c r="BD1" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="BD1" s="11" t="s">
+      <c r="BE1" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="BE1" s="11" t="s">
+      <c r="BF1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="BF1" s="11" t="s">
+      <c r="BG1" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="BG1" s="11" t="s">
+      <c r="BH1" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="BH1" s="11" t="s">
+      <c r="BI1" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="BI1" s="11" t="s">
+      <c r="BJ1" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="BJ1" s="11" t="s">
+      <c r="BK1" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="BK1" s="11" t="s">
+      <c r="BL1" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="BL1" s="11" t="s">
+      <c r="BM1" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="BM1" s="11" t="s">
+      <c r="BN1" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="BN1" s="11" t="s">
+      <c r="BO1" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="BO1" s="11" t="s">
+      <c r="BP1" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="BP1" s="11" t="s">
+      <c r="BQ1" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="BQ1" s="11" t="s">
+      <c r="BR1" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="BR1" s="11" t="s">
+      <c r="BS1" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="BS1" s="11" t="s">
+      <c r="BT1" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="BT1" s="11" t="s">
+      <c r="BU1" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="BU1" s="11" t="s">
+      <c r="BV1" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="BV1" s="11" t="s">
+      <c r="BW1" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="BW1" s="11" t="s">
+      <c r="BX1" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="BX1" s="11" t="s">
+      <c r="BY1" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="BY1" s="11" t="s">
+      <c r="BZ1" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="BZ1" s="11" t="s">
+      <c r="CA1" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="CA1" s="11" t="s">
+      <c r="CB1" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="CB1" s="11" t="s">
+      <c r="CC1" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="CC1" s="11" t="s">
+      <c r="CD1" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="CD1" s="11" t="s">
+      <c r="CE1" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="CE1" s="11" t="s">
+      <c r="CF1" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="CF1" s="11" t="s">
+      <c r="CG1" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="CG1" s="11" t="s">
+      <c r="CH1" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="CH1" s="11" t="s">
+      <c r="CI1" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="CI1" s="11" t="s">
+      <c r="CJ1" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="CJ1" s="11" t="s">
+      <c r="CK1" s="45" t="s">
         <v>92</v>
       </c>
-      <c r="CK1" s="11" t="s">
+      <c r="CL1" s="45" t="s">
         <v>93</v>
       </c>
-      <c r="CL1" s="11" t="s">
+      <c r="CM1" s="45" t="s">
         <v>94</v>
       </c>
-      <c r="CM1" s="11" t="s">
+      <c r="CN1" s="45" t="s">
         <v>95</v>
       </c>
-      <c r="CN1" s="11" t="s">
+      <c r="CO1" s="45" t="s">
         <v>96</v>
       </c>
-      <c r="CO1" s="11" t="s">
+      <c r="CP1" s="45" t="s">
         <v>97</v>
       </c>
-      <c r="CP1" s="11" t="s">
+      <c r="CQ1" s="45" t="s">
         <v>98</v>
       </c>
-      <c r="CQ1" s="11" t="s">
+      <c r="CR1" s="45" t="s">
         <v>99</v>
       </c>
-      <c r="CR1" s="11" t="s">
+      <c r="CS1" s="45" t="s">
         <v>100</v>
       </c>
-      <c r="CS1" s="11" t="s">
+      <c r="CT1" s="45" t="s">
         <v>101</v>
       </c>
-      <c r="CT1" s="11" t="s">
+      <c r="CU1" s="45" t="s">
         <v>102</v>
       </c>
-      <c r="CU1" s="11" t="s">
+      <c r="CV1" s="45" t="s">
+        <v>1</v>
+      </c>
+      <c r="CW1" s="45" t="s">
+        <v>2</v>
+      </c>
+      <c r="CX1" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="CV1" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="CW1" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="CX1" s="11" t="s">
+      <c r="CY1" s="45" t="s">
         <v>104</v>
       </c>
-      <c r="CY1" s="11" t="s">
+      <c r="CZ1" s="45" t="s">
         <v>105</v>
       </c>
-      <c r="CZ1" s="11" t="s">
+      <c r="DA1" s="45" t="s">
         <v>106</v>
       </c>
-      <c r="DA1" s="11" t="s">
+      <c r="DB1" s="45" t="s">
         <v>107</v>
       </c>
-      <c r="DB1" s="11" t="s">
+      <c r="DC1" s="45" t="s">
         <v>108</v>
       </c>
-      <c r="DC1" s="11" t="s">
+      <c r="DD1" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="DD1" s="11" t="s">
+      <c r="DE1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="DE1" s="11" t="s">
+      <c r="DF1" s="45" t="s">
         <v>111</v>
       </c>
-      <c r="DF1" s="11" t="s">
+      <c r="DG1" s="45" t="s">
         <v>112</v>
       </c>
-      <c r="DG1" s="11" t="s">
+      <c r="DH1" s="45" t="s">
         <v>113</v>
       </c>
-      <c r="DH1" s="11" t="s">
+      <c r="DI1" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="DI1" s="11" t="s">
+      <c r="DJ1" s="45" t="s">
         <v>115</v>
       </c>
-      <c r="DJ1" s="11" t="s">
+      <c r="DK1" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="DK1" s="11" t="s">
+      <c r="DL1" s="45" t="s">
         <v>117</v>
       </c>
-      <c r="DL1" s="11" t="s">
+      <c r="DM1" s="45" t="s">
         <v>118</v>
       </c>
-      <c r="DM1" s="11" t="s">
+      <c r="DN1" s="45" t="s">
         <v>119</v>
       </c>
-      <c r="DN1" s="11" t="s">
+      <c r="DO1" s="45" t="s">
         <v>120</v>
       </c>
-      <c r="DO1" s="11" t="s">
+      <c r="DP1" s="45" t="s">
         <v>121</v>
       </c>
-      <c r="DP1" s="11" t="s">
+      <c r="DQ1" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="DQ1" s="4" t="s">
+      <c r="DR1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="DR1" s="4" t="s">
+      <c r="DS1" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="DS1" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:123" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>127</v>
       </c>
       <c r="C2" s="1">
         <v>1</v>
@@ -2023,19 +2183,19 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>173</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>174</v>
+        <v>129</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>175</v>
+        <v>130</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J2" s="2">
         <v>34700</v>
@@ -2044,37 +2204,37 @@
         <v>0</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="M2" s="1">
         <v>9876500000</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="O2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>137</v>
+        <v>168</v>
       </c>
       <c r="W2" s="1" t="s">
         <v>138</v>
@@ -2083,7 +2243,7 @@
         <v>25569</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>139</v>
+        <v>169</v>
       </c>
       <c r="Z2" s="1">
         <v>91</v>
@@ -2092,43 +2252,43 @@
         <v>454545245</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="AC2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="AF2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>5</v>
+        <v>170</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>141</v>
+        <v>171</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>142</v>
+        <v>172</v>
       </c>
       <c r="AJ2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AK2" s="1" t="s">
-        <v>143</v>
+        <v>173</v>
       </c>
       <c r="AL2" s="1" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="AM2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AN2" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="AO2" s="1">
         <v>3</v>
@@ -2140,19 +2300,19 @@
         <v>562</v>
       </c>
       <c r="AR2" s="1" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="AS2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AT2" s="2">
         <v>46054</v>
       </c>
       <c r="AU2" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="AV2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AW2" s="2">
         <v>46023</v>
@@ -2161,10 +2321,10 @@
         <v>46388</v>
       </c>
       <c r="AY2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="AZ2" s="1" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="BA2" s="1">
         <v>0</v>
@@ -2173,16 +2333,16 @@
         <v>46023</v>
       </c>
       <c r="BC2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BD2" s="1" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="BE2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BF2" s="1" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="BG2" s="1" t="s">
         <v>0</v>
@@ -2194,13 +2354,13 @@
         <v>47484</v>
       </c>
       <c r="BJ2" s="1" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="BK2" s="1" t="s">
-        <v>150</v>
+        <v>175</v>
       </c>
       <c r="BL2" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="BM2" s="2">
         <v>47484</v>
@@ -2215,19 +2375,19 @@
         <v>49644</v>
       </c>
       <c r="BQ2" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="BR2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="BS2" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="BT2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="BU2" s="1" t="s">
-        <v>154</v>
+        <v>176</v>
       </c>
       <c r="BV2" s="2">
         <v>49310</v>
@@ -2239,10 +2399,10 @@
         <v>51136</v>
       </c>
       <c r="BY2" s="1" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="BZ2" s="1" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="CA2" s="1" t="s">
         <v>0</v>
@@ -2251,19 +2411,19 @@
         <v>46023</v>
       </c>
       <c r="CC2" s="1" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="CD2" s="1" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="CE2" s="2">
         <v>46023</v>
       </c>
       <c r="CF2" s="1" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="CG2" s="1" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="CH2" s="2">
         <v>46023</v>
@@ -2275,7 +2435,7 @@
         <v>4</v>
       </c>
       <c r="CK2" s="1" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="CL2" s="2">
         <v>45658</v>
@@ -2290,22 +2450,22 @@
         <v>85</v>
       </c>
       <c r="CP2" s="1" t="s">
-        <v>160</v>
+        <v>154</v>
       </c>
       <c r="CQ2" s="1">
         <v>90</v>
       </c>
       <c r="CR2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="CS2" s="1" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
       <c r="CT2" s="1" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
       <c r="CU2" s="1" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="CV2" s="2">
         <v>45292</v>
@@ -2314,13 +2474,13 @@
         <v>45658</v>
       </c>
       <c r="CX2" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="CY2" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="DA2" s="1">
         <v>88</v>
@@ -2329,16 +2489,16 @@
         <v>45658</v>
       </c>
       <c r="DC2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="DD2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="DE2" s="1" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="DF2" s="1" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="DG2" s="2">
         <v>44927</v>
@@ -2350,22 +2510,22 @@
         <v>46023</v>
       </c>
       <c r="DJ2" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="DK2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="DL2" s="1" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="DM2" s="1" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="DN2" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="DO2" s="12" t="s">
-        <v>172</v>
+        <v>137</v>
+      </c>
+      <c r="DO2" s="46" t="s">
+        <v>166</v>
       </c>
       <c r="DP2" s="2">
         <v>46023</v>
@@ -2374,10 +2534,10 @@
         <v>4554</v>
       </c>
       <c r="DR2" s="1" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>